<commit_message>
define S004 Scenario Coolmate Test
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-003.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-003.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncbao\Downloads\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaoNguyen\OneDrive\Máy tính\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6319262E-D6D8-4ECE-8F1B-9EEA153154CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COOLMATE-003" sheetId="1" r:id="rId1"/>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -523,26 +524,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -594,7 +595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -620,7 +621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="69" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -646,7 +647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Revert "define S004 Scenario Coolmate Test"
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-003.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-003.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaoNguyen\OneDrive\Máy tính\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncbao\Downloads\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6319262E-D6D8-4ECE-8F1B-9EEA153154CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="COOLMATE-003" sheetId="1" r:id="rId1"/>
@@ -107,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -524,26 +523,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,7 +568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -595,7 +594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -621,7 +620,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="69" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -647,7 +646,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "define S004 Scenario Coolmate Test""
This reverts commit e9c007358da7c24382906d228d614ed6a727daf4.
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-003.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-003.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncbao\Downloads\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaoNguyen\OneDrive\Máy tính\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6319262E-D6D8-4ECE-8F1B-9EEA153154CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COOLMATE-003" sheetId="1" r:id="rId1"/>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -523,26 +524,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -594,7 +595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -620,7 +621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="69" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -646,7 +647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>

</xml_diff>